<commit_message>
Adding rating logic, bowling and batting and scorecard creation logic
</commit_message>
<xml_diff>
--- a/project/temp/RatingTesting.xlsx
+++ b/project/temp/RatingTesting.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ystrategists-my.sharepoint.com/personal/shyam_rangapure_metyis_com/Documents/Documenten/Side Projects/Dream11/project/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1318" documentId="8_{96C61FCE-C6EC-45E1-838C-3015975C7AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{133DC13A-9CA0-4341-B2CF-90BA1A2572DF}"/>
+  <xr:revisionPtr revIDLastSave="1396" documentId="8_{96C61FCE-C6EC-45E1-838C-3015975C7AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3543979F-8267-46ED-8186-4367DB6CCB41}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="504" xr2:uid="{4278B6C9-FDEA-4D23-B6FA-D5A427574231}"/>
   </bookViews>
   <sheets>
     <sheet name="Scorecard" sheetId="1" r:id="rId1"/>
-    <sheet name="ODI resource sheet" sheetId="3" r:id="rId2"/>
-    <sheet name="Partnerships" sheetId="2" r:id="rId3"/>
-    <sheet name="T20 resource sheet" sheetId="5" r:id="rId4"/>
-    <sheet name="T20 resource sheet EXP" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="ODI resource sheet" sheetId="3" r:id="rId3"/>
+    <sheet name="Partnerships" sheetId="2" r:id="rId4"/>
+    <sheet name="T20 resource sheet" sheetId="5" r:id="rId5"/>
+    <sheet name="T20 resource sheet EXP" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="161">
   <si>
     <t>Jaiswal</t>
   </si>
@@ -568,6 +570,21 @@
   <si>
     <t>Runs/Ball/range</t>
   </si>
+  <si>
+    <t>Bowlers</t>
+  </si>
+  <si>
+    <t>Dotballs</t>
+  </si>
+  <si>
+    <t>Wickets</t>
+  </si>
+  <si>
+    <t>WicketWeightage</t>
+  </si>
+  <si>
+    <t>Runs given (Economy)</t>
+  </si>
 </sst>
 </file>
 
@@ -702,15 +719,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC1553B6-D3D9-41CE-B753-72CD14B8F659}" name="Table1" displayName="Table1" ref="A1:AF19" totalsRowCount="1">
-  <autoFilter ref="A1:AF18" xr:uid="{EC1553B6-D3D9-41CE-B753-72CD14B8F659}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="AUS"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AF18">
-    <sortCondition ref="A1:A18"/>
+  <autoFilter ref="A1:AF18" xr:uid="{EC1553B6-D3D9-41CE-B753-72CD14B8F659}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF18">
+    <sortCondition descending="1" ref="AF1:AF18"/>
   </sortState>
   <tableColumns count="32">
     <tableColumn id="14" xr3:uid="{FF79C271-5126-491C-BB01-A84123EB7B8C}" name="Batting Order"/>
@@ -1237,17 +1248,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8413B3B0-8DCD-4EAA-BF25-3E9F9A809CB0}">
-  <dimension ref="A1:AU45"/>
+  <dimension ref="A1:AU44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AN34" sqref="AN34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="13" width="12" customWidth="1"/>
     <col min="14" max="14" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="9.33203125" customWidth="1"/>
@@ -1377,7 +1388,7 @@
         <v>33.764705882352942</v>
       </c>
     </row>
-    <row r="2" spans="1:42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1439,7 +1450,7 @@
       </c>
       <c r="T2">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>28.148148148148167</v>
+        <v>32.631578947368425</v>
       </c>
       <c r="U2">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
@@ -1507,10 +1518,10 @@
       </c>
       <c r="AP2">
         <f>AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]])*100</f>
-        <v>105.18518518518518</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" hidden="1" x14ac:dyDescent="0.3">
+        <v>100.70175438596492</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1575,7 +1586,7 @@
       </c>
       <c r="T3">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>19.814814814814824</v>
+        <v>24.298245614035082</v>
       </c>
       <c r="U3">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
@@ -1647,117 +1658,117 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="E4">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>300</v>
+        <v>222</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I4">
-        <v>222</v>
+        <v>53</v>
       </c>
       <c r="J4">
-        <v>100</v>
+        <v>58.2</v>
       </c>
       <c r="K4">
-        <v>58.2</v>
+        <v>11.1</v>
       </c>
       <c r="L4">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.25518341307814996</v>
+        <v>0.92002830856334039</v>
       </c>
       <c r="M4">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>125.87204999999999</v>
+        <v>133.63447500000001</v>
       </c>
       <c r="N4">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="O4">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>32.120459330143539</v>
+        <v>122.94750000000001</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>6.69</v>
       </c>
       <c r="Q4">
-        <v>6.69</v>
+        <v>6.56</v>
       </c>
       <c r="R4">
-        <f>D4*100/E4</f>
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>88.461538461538467</v>
       </c>
       <c r="S4">
         <f>D4-AVERAGE(Table1[Runs])</f>
-        <v>6.235294117647058</v>
+        <v>81.235294117647058</v>
       </c>
       <c r="T4">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>19.814814814814824</v>
+        <v>-12.240215924426451</v>
       </c>
       <c r="U4">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>1.2453122039404301</v>
+        <v>0.93535858801520966</v>
       </c>
       <c r="V4">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0.84787213885305868</v>
+        <v>1.3510735160219696</v>
       </c>
       <c r="W4">
         <v>-30</v>
       </c>
       <c r="X4">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Y4">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Z4">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AA4">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB4">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>18.75</v>
+        <v>30</v>
       </c>
       <c r="AC4">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>6.875</v>
+        <v>5</v>
       </c>
       <c r="AD4">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>37.5</v>
+        <v>30</v>
       </c>
       <c r="AE4">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>45</v>
+        <v>52.5</v>
       </c>
       <c r="AF4">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>70.625</v>
+        <v>87.5</v>
       </c>
       <c r="AO4" t="s">
         <v>32</v>
@@ -1766,7 +1777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>5.82</v>
       </c>
       <c r="R5">
-        <f>D5*100/E5</f>
+        <f t="shared" si="0"/>
         <v>83.333333333333329</v>
       </c>
       <c r="S5">
@@ -1828,7 +1839,7 @@
       </c>
       <c r="T5">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-21.851851851851848</v>
+        <v>-17.368421052631589</v>
       </c>
       <c r="U5">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
@@ -1886,19 +1897,19 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1907,96 +1918,96 @@
         <v>300</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>292</v>
+        <v>222</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6">
-        <v>92.3</v>
+        <v>58.2</v>
       </c>
       <c r="L6">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.12987012987012983</v>
+        <v>0.25518341307814996</v>
       </c>
       <c r="M6">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>24.647700000000007</v>
+        <v>125.87204999999999</v>
       </c>
       <c r="N6">
         <v>47</v>
       </c>
       <c r="O6">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>3.2010000000000001</v>
+        <v>32.120459330143539</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1.5</v>
+        <v>6.69</v>
       </c>
       <c r="R6">
-        <f>D6*100/E6</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>125</v>
       </c>
       <c r="S6">
         <f>D6-AVERAGE(Table1[Runs])</f>
-        <v>-33.764705882352942</v>
+        <v>6.235294117647058</v>
       </c>
       <c r="T6">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-105.18518518518518</v>
+        <v>24.298245614035082</v>
       </c>
       <c r="U6">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0</v>
+        <v>1.2453122039404301</v>
       </c>
       <c r="V6">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0</v>
+        <v>0.84787213885305868</v>
       </c>
       <c r="W6">
         <v>-30</v>
       </c>
       <c r="X6">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Y6">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="Z6">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AA6">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="AB6">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>1.875</v>
+        <v>18.75</v>
       </c>
       <c r="AC6">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>0.625</v>
+        <v>6.875</v>
       </c>
       <c r="AD6">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>3.75</v>
+        <v>37.5</v>
       </c>
       <c r="AE6">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>3.75</v>
+        <v>45</v>
       </c>
       <c r="AF6">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>6.25</v>
+        <v>70.625</v>
       </c>
       <c r="AI6">
         <v>300</v>
@@ -2010,117 +2021,117 @@
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>275</v>
+        <v>143</v>
       </c>
       <c r="J7">
-        <v>92.3</v>
+        <v>69</v>
       </c>
       <c r="K7">
-        <v>82.4</v>
+        <v>41.5</v>
       </c>
       <c r="L7">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.23569023569023589</v>
+        <v>0.38787878787878788</v>
       </c>
       <c r="M7">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>31.68989999999997</v>
+        <v>78.024375000000006</v>
       </c>
       <c r="N7">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="O7">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>7.4689999999999994</v>
+        <v>30.264000000000003</v>
       </c>
       <c r="P7">
-        <v>1.5</v>
+        <v>6.09</v>
       </c>
       <c r="Q7">
-        <v>3.84</v>
+        <v>6.53</v>
       </c>
       <c r="R7">
-        <f>D7*100/E7</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>140.625</v>
       </c>
       <c r="S7">
         <f>D7-AVERAGE(Table1[Runs])</f>
-        <v>-33.764705882352942</v>
+        <v>11.235294117647058</v>
       </c>
       <c r="T7">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-105.18518518518518</v>
+        <v>39.923245614035082</v>
       </c>
       <c r="U7">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0</v>
+        <v>1.486915146708961</v>
       </c>
       <c r="V7">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0</v>
+        <v>0.63441712926249005</v>
       </c>
       <c r="W7">
         <v>-30</v>
       </c>
       <c r="X7">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="Y7">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Z7">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="AA7">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AB7">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>1.875</v>
+        <v>22.5</v>
       </c>
       <c r="AC7">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>0.625</v>
+        <v>8.125</v>
       </c>
       <c r="AD7">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>3.75</v>
+        <v>48.75</v>
       </c>
       <c r="AE7">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>3.75</v>
+        <v>37.5</v>
       </c>
       <c r="AF7">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>6.25</v>
+        <v>68.125</v>
       </c>
       <c r="AI7">
         <v>240</v>
@@ -2195,7 +2206,7 @@
         <v>6.09</v>
       </c>
       <c r="R8">
-        <f>D8*100/E8</f>
+        <f t="shared" si="0"/>
         <v>146.42857142857142</v>
       </c>
       <c r="S8">
@@ -2204,7 +2215,7 @@
       </c>
       <c r="T8">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>41.24338624338624</v>
+        <v>45.726817042606498</v>
       </c>
       <c r="U8">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
@@ -2259,114 +2270,111 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9">
-        <v>234</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="I9">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>69</v>
+        <v>51.5</v>
       </c>
       <c r="K9">
-        <v>41.5</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.38787878787878788</v>
+        <v>0.38834951456310679</v>
       </c>
       <c r="M9">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>78.024375000000006</v>
+        <v>146.11837500000001</v>
       </c>
       <c r="N9">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="O9">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>30.264000000000003</v>
+        <v>56.745000000000005</v>
       </c>
       <c r="P9">
-        <v>6.09</v>
+        <v>5.82</v>
       </c>
       <c r="Q9">
-        <v>6.53</v>
+        <v>5.8</v>
       </c>
       <c r="R9">
-        <f>D9*100/E9</f>
-        <v>140.625</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="S9">
         <f>D9-AVERAGE(Table1[Runs])</f>
-        <v>11.235294117647058</v>
+        <v>-3.764705882352942</v>
       </c>
       <c r="T9">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>35.439814814814824</v>
+        <v>-50.701754385964918</v>
       </c>
       <c r="U9">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>1.486915146708961</v>
+        <v>0.52868094105207508</v>
       </c>
       <c r="V9">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0.63441712926249005</v>
+        <v>0.83475938060853938</v>
       </c>
       <c r="W9">
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="X9">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Y9">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="Z9">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="AA9">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB9">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>22.5</v>
+        <v>16.875</v>
       </c>
       <c r="AC9">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>8.125</v>
+        <v>2.5</v>
       </c>
       <c r="AD9">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>48.75</v>
+        <v>15</v>
       </c>
       <c r="AE9">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>37.5</v>
+        <v>41.25</v>
       </c>
       <c r="AF9">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>68.125</v>
+        <v>60.625</v>
       </c>
       <c r="AO9" t="s">
         <v>115</v>
@@ -2375,119 +2383,122 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="10" spans="1:42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>30</v>
-      </c>
-      <c r="E10">
-        <v>60</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
       <c r="G10">
-        <v>130</v>
+        <v>143</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="J10">
-        <v>51.5</v>
+        <v>41.5</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="L10">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.38834951456310679</v>
+        <v>0.17948717948717949</v>
       </c>
       <c r="M10">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>146.11837500000001</v>
+        <v>36.884250000000002</v>
       </c>
       <c r="N10">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="O10">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>56.745000000000005</v>
+        <v>6.6202500000000004</v>
       </c>
       <c r="P10">
-        <v>5.82</v>
+        <v>6.53</v>
       </c>
       <c r="Q10">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="R10">
-        <f>D10*100/E10</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>285.71428571428572</v>
       </c>
       <c r="S10">
         <f>D10-AVERAGE(Table1[Runs])</f>
-        <v>-3.764705882352942</v>
+        <v>-13.764705882352942</v>
       </c>
       <c r="T10">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-55.185185185185176</v>
+        <v>185.01253132832079</v>
       </c>
       <c r="U10">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0.52868094105207508</v>
+        <v>3.0210339488690003</v>
       </c>
       <c r="V10">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0.83475938060853938</v>
+        <v>0.29784841749412677</v>
       </c>
       <c r="W10">
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="X10">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Y10">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="AA10">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AB10">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>16.875</v>
+        <v>15</v>
       </c>
       <c r="AC10">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="AD10">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="AE10">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>41.25</v>
+        <v>26.25</v>
       </c>
       <c r="AF10">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>60.625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" hidden="1" x14ac:dyDescent="0.3">
+        <v>51.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2543,7 +2554,7 @@
         <v>9</v>
       </c>
       <c r="R11">
-        <f>D11*100/E11</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="S11">
@@ -2552,7 +2563,7 @@
       </c>
       <c r="T11">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-5.1851851851851762</v>
+        <v>-0.70175438596491801</v>
       </c>
       <c r="U11">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
@@ -2610,117 +2621,117 @@
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G12">
-        <v>222</v>
+        <v>80</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I12">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="J12">
-        <v>58.2</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="K12">
-        <v>11.1</v>
+        <v>4.7</v>
       </c>
       <c r="L12">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.92002830856334039</v>
+        <v>0.15659955257270691</v>
       </c>
       <c r="M12">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>133.63447500000001</v>
+        <v>42.275025000000007</v>
       </c>
       <c r="N12">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="O12">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>122.94750000000001</v>
+        <v>6.6202500000000004</v>
       </c>
       <c r="P12">
-        <v>6.69</v>
+        <v>6.55</v>
       </c>
       <c r="Q12">
-        <v>6.56</v>
+        <v>6.49</v>
       </c>
       <c r="R12">
-        <f>D12*100/E12</f>
-        <v>88.461538461538467</v>
+        <f t="shared" si="0"/>
+        <v>142.85714285714286</v>
       </c>
       <c r="S12">
         <f>D12-AVERAGE(Table1[Runs])</f>
-        <v>81.235294117647058</v>
+        <v>-23.764705882352942</v>
       </c>
       <c r="T12">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-16.723646723646709</v>
+        <v>42.155388471177943</v>
       </c>
       <c r="U12">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0.93535858801520966</v>
+        <v>1.5105169744345002</v>
       </c>
       <c r="V12">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>1.3510735160219696</v>
+        <v>0.16521279407877346</v>
       </c>
       <c r="W12">
         <v>-30</v>
       </c>
       <c r="X12">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y12">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="Z12">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="AA12">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="AB12">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>30</v>
+        <v>11.25</v>
       </c>
       <c r="AC12">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>5</v>
+        <v>8.75</v>
       </c>
       <c r="AD12">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>30</v>
+        <v>52.5</v>
       </c>
       <c r="AE12">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>52.5</v>
+        <v>18.75</v>
       </c>
       <c r="AF12">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>87.5</v>
+        <v>38.75</v>
       </c>
       <c r="AI12">
         <v>0</v>
@@ -2738,7 +2749,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2794,7 +2805,7 @@
         <v>6.38</v>
       </c>
       <c r="R13">
-        <f>D13*100/E13</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="S13">
@@ -2803,7 +2814,7 @@
       </c>
       <c r="T13">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-55.185185185185176</v>
+        <v>-50.701754385964918</v>
       </c>
       <c r="U13">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
@@ -2855,117 +2866,117 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="J14">
-        <v>41.5</v>
+        <v>11.1</v>
       </c>
       <c r="K14">
-        <v>28.5</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.17948717948717949</v>
+        <v>0.24024024024024027</v>
       </c>
       <c r="M14">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>36.884250000000002</v>
+        <v>31.493475</v>
       </c>
       <c r="N14">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="O14">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>6.6202500000000004</v>
+        <v>7.5660000000000007</v>
       </c>
       <c r="P14">
-        <v>6.53</v>
+        <v>6.56</v>
       </c>
       <c r="Q14">
-        <v>6.5</v>
+        <v>6.3109999999999999</v>
       </c>
       <c r="R14">
-        <f>D14*100/E14</f>
-        <v>285.71428571428572</v>
+        <f t="shared" si="0"/>
+        <v>62.5</v>
       </c>
       <c r="S14">
         <f>D14-AVERAGE(Table1[Runs])</f>
-        <v>-13.764705882352942</v>
+        <v>-28.764705882352942</v>
       </c>
       <c r="T14">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>180.52910052910056</v>
+        <v>-38.201754385964918</v>
       </c>
       <c r="U14">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>3.0210339488690003</v>
+        <v>0.66085117631509382</v>
       </c>
       <c r="V14">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0.29784841749412677</v>
+        <v>9.9751120953221695E-2</v>
       </c>
       <c r="W14">
         <v>-30</v>
       </c>
       <c r="X14">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="Y14">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="Z14">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="AA14">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="AB14">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="AC14">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>10</v>
+        <v>3.125</v>
       </c>
       <c r="AD14">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>60</v>
+        <v>18.75</v>
       </c>
       <c r="AE14">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>26.25</v>
+        <v>11.25</v>
       </c>
       <c r="AF14">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>51.25</v>
+        <v>21.875</v>
       </c>
       <c r="AI14">
         <v>60</v>
@@ -2986,62 +2997,59 @@
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G15">
-        <v>96</v>
-      </c>
-      <c r="H15">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="I15">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J15">
-        <v>28.5</v>
+        <v>4.7</v>
       </c>
       <c r="K15">
-        <v>19.600000000000001</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.22471910112359555</v>
+        <v>0.70921985815602828</v>
       </c>
       <c r="M15">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>25.251524999999997</v>
+        <v>13.335075000000002</v>
       </c>
       <c r="N15">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="O15">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>5.674500000000001</v>
+        <v>9.4574999999999996</v>
       </c>
       <c r="P15">
-        <v>6.5</v>
+        <v>6.49</v>
       </c>
       <c r="Q15">
-        <v>6.55</v>
+        <v>6.3109999999999999</v>
       </c>
       <c r="R15">
-        <f>D15*100/E15</f>
-        <v>66.666666666666671</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="S15">
         <f>D15-AVERAGE(Table1[Runs])</f>
@@ -3049,15 +3057,15 @@
       </c>
       <c r="T15">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-38.518518518518505</v>
+        <v>-60.701754385964918</v>
       </c>
       <c r="U15">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0.70490792140276659</v>
+        <v>0.42294475284166005</v>
       </c>
       <c r="V15">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>7.0490792140276662E-2</v>
+        <v>0.1031572567906488</v>
       </c>
       <c r="W15">
         <v>-30</v>
@@ -3068,15 +3076,15 @@
       </c>
       <c r="Y15">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Z15">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AA15">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB15">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
@@ -3084,19 +3092,19 @@
       </c>
       <c r="AC15">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>3.75</v>
+        <v>1.25</v>
       </c>
       <c r="AD15">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>22.5</v>
+        <v>7.5</v>
       </c>
       <c r="AE15">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="AF15">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>16.875</v>
+        <v>21.875</v>
       </c>
       <c r="AI15">
         <v>120</v>
@@ -3116,117 +3124,117 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>96</v>
+      </c>
+      <c r="H16">
         <v>7</v>
       </c>
-      <c r="F16">
-        <v>7</v>
-      </c>
-      <c r="G16">
+      <c r="I16">
         <v>80</v>
       </c>
-      <c r="H16">
-        <v>9</v>
-      </c>
-      <c r="I16">
-        <v>41</v>
-      </c>
       <c r="J16">
+        <v>28.5</v>
+      </c>
+      <c r="K16">
         <v>19.600000000000001</v>
-      </c>
-      <c r="K16">
-        <v>4.7</v>
       </c>
       <c r="L16">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.15659955257270691</v>
+        <v>0.22471910112359555</v>
       </c>
       <c r="M16">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>42.275025000000007</v>
+        <v>25.251524999999997</v>
       </c>
       <c r="N16">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O16">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>6.6202500000000004</v>
+        <v>5.674500000000001</v>
       </c>
       <c r="P16">
+        <v>6.5</v>
+      </c>
+      <c r="Q16">
         <v>6.55</v>
       </c>
-      <c r="Q16">
-        <v>6.49</v>
-      </c>
       <c r="R16">
-        <f>D16*100/E16</f>
-        <v>142.85714285714286</v>
+        <f t="shared" si="0"/>
+        <v>66.666666666666671</v>
       </c>
       <c r="S16">
         <f>D16-AVERAGE(Table1[Runs])</f>
-        <v>-23.764705882352942</v>
+        <v>-29.764705882352942</v>
       </c>
       <c r="T16">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>37.671957671957685</v>
+        <v>-34.035087719298247</v>
       </c>
       <c r="U16">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>1.5105169744345002</v>
+        <v>0.70490792140276659</v>
       </c>
       <c r="V16">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0.16521279407877346</v>
+        <v>7.0490792140276662E-2</v>
       </c>
       <c r="W16">
         <v>-30</v>
       </c>
       <c r="X16">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Y16">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="Z16">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AA16">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AB16">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>11.25</v>
+        <v>5.625</v>
       </c>
       <c r="AC16">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>8.75</v>
+        <v>3.75</v>
       </c>
       <c r="AD16">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>52.5</v>
+        <v>22.5</v>
       </c>
       <c r="AE16">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>18.75</v>
+        <v>7.5</v>
       </c>
       <c r="AF16">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>38.75</v>
+        <v>16.875</v>
       </c>
       <c r="AI16">
         <v>210</v>
@@ -3246,229 +3254,232 @@
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>53</v>
+        <v>300</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>30</v>
+        <v>292</v>
       </c>
       <c r="J17">
-        <v>11.1</v>
+        <v>100</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>92.3</v>
       </c>
       <c r="L17">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.24024024024024027</v>
+        <v>0.12987012987012983</v>
       </c>
       <c r="M17">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>31.493475</v>
+        <v>24.647700000000007</v>
       </c>
       <c r="N17">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="O17">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>7.5660000000000007</v>
+        <v>3.2010000000000001</v>
       </c>
       <c r="P17">
-        <v>6.56</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>6.3109999999999999</v>
+        <v>1.5</v>
       </c>
       <c r="R17">
-        <f>D17*100/E17</f>
-        <v>62.5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="S17">
         <f>D17-AVERAGE(Table1[Runs])</f>
-        <v>-28.764705882352942</v>
+        <v>-33.764705882352942</v>
       </c>
       <c r="T17">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-42.685185185185176</v>
+        <v>-100.70175438596492</v>
       </c>
       <c r="U17">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0.66085117631509382</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>9.9751120953221695E-2</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <v>-30</v>
       </c>
       <c r="X17">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Y17">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z17">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="AA17">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AB17">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>7.5</v>
+        <v>1.875</v>
       </c>
       <c r="AC17">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>3.125</v>
+        <v>0.625</v>
       </c>
       <c r="AD17">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>18.75</v>
+        <v>3.75</v>
       </c>
       <c r="AE17">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>11.25</v>
+        <v>3.75</v>
       </c>
       <c r="AF17">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>21.875</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>41</v>
+        <v>292</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>30</v>
+        <v>275</v>
       </c>
       <c r="J18">
-        <v>4.7</v>
+        <v>92.3</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>82.4</v>
       </c>
       <c r="L18">
         <f>Table1[[#This Row],[Balls Faced]]/((Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*3)</f>
-        <v>0.70921985815602828</v>
+        <v>0.23569023569023589</v>
       </c>
       <c r="M18">
         <f>(IF(Table1[[#This Row],[InResource]]&gt;80,Table1[[#This Row],[InResource]]-MAX(Table1[[#This Row],[OutResource]],80),0) * $AM$2) + IF(Table1[[#This Row],[OutResource]]&lt;80,IF(Table1[[#This Row],[InResource]]&lt;80, (Table1[[#This Row],[InResource]]-Table1[[#This Row],[OutResource]])*$AM$3, (80 - Table1[[#This Row],[OutResource]])*$AM$3),0)</f>
-        <v>13.335075000000002</v>
+        <v>31.68989999999997</v>
       </c>
       <c r="N18">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="O18">
         <f>Table1[[#This Row],[total resources inning duration]]*Table1[[#This Row],[%resource used]]</f>
-        <v>9.4574999999999996</v>
+        <v>7.4689999999999994</v>
       </c>
       <c r="P18">
-        <v>6.49</v>
+        <v>1.5</v>
       </c>
       <c r="Q18">
-        <v>6.3109999999999999</v>
+        <v>3.84</v>
       </c>
       <c r="R18">
-        <f>D18*100/E18</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="S18">
         <f>D18-AVERAGE(Table1[Runs])</f>
-        <v>-29.764705882352942</v>
+        <v>-33.764705882352942</v>
       </c>
       <c r="T18">
         <f>Table1[[#This Row],[SR]]-(100*AVERAGE(Table1[[#Totals],[Runs]]/Table1[[#Totals],[Balls Faced]]))</f>
-        <v>-65.185185185185176</v>
+        <v>-100.70175438596492</v>
       </c>
       <c r="U18">
         <f>Table1[[#This Row],[Runs]]/Table1[[#This Row],[Expected result (Runs)]]</f>
-        <v>0.42294475284166005</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <f>(Table1[[#This Row],[Balls Faced]]*Table1[[#This Row],[Runs]])/(Table1[[#This Row],[Exp Resources utilization (balls)]]*Table1[[#This Row],[Expected result (Runs)]])</f>
-        <v>0.1031572567906488</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>-30</v>
       </c>
       <c r="X18">
         <f>RANK(Table1[[#This Row],[Metric1]],Table1[Metric1])</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Y18">
         <f>RANK(Table1[[#This Row],[Metric2]],Table1[Metric2])</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z18">
         <f>RANK(Table1[[#This Row],[Metric3]],Table1[Metric3])</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AA18">
         <f>RANK(Table1[[#This Row],[Metric3_Enhanced]],Table1[Metric3_Enhanced])</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AB18">
         <f>$AP$3-(($AP$3/($AP$7-1)) * (Table1[[#This Row],[M1Rank]]-1))</f>
-        <v>5.625</v>
+        <v>1.875</v>
       </c>
       <c r="AC18">
         <f>$AP$4-(($AP$4/($AP$7-1)) * (Table1[[#This Row],[M2Rank]]-1))</f>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="AD18">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3Rank]]-1))</f>
-        <v>7.5</v>
+        <v>3.75</v>
       </c>
       <c r="AE18">
         <f>$AP$5-(($AP$5/($AP$7-1)) * (Table1[[#This Row],[M3.1Rank]]-1))</f>
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="AF18">
         <f>Table1[[#This Row],[Wt.Metric1]]+Table1[[#This Row],[WtMetric2]]+Table1[[#This Row],[WtMetric3.1]]</f>
-        <v>21.875</v>
+        <v>6.25</v>
       </c>
       <c r="AJ18">
         <v>307</v>
@@ -3484,15 +3495,15 @@
       </c>
       <c r="D19">
         <f>SUBTOTAL(109,Table1[Runs])</f>
-        <v>284</v>
+        <v>574</v>
       </c>
       <c r="E19">
         <f>SUBTOTAL(109,Table1[Balls Faced])</f>
-        <v>270</v>
+        <v>570</v>
       </c>
       <c r="N19">
         <f>SUBTOTAL(109,Table1[Exp Resources utilization (balls)])</f>
-        <v>684</v>
+        <v>962</v>
       </c>
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.3">
@@ -3680,17 +3691,119 @@
         <v>307</v>
       </c>
     </row>
-    <row r="44" spans="38:39" x14ac:dyDescent="0.3">
-      <c r="AL44">
-        <v>239</v>
-      </c>
-      <c r="AM44">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="45" spans="38:39" x14ac:dyDescent="0.3">
-      <c r="AM45">
-        <v>60</v>
+    <row r="33" spans="35:45" x14ac:dyDescent="0.3">
+      <c r="AN33">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="35:45" x14ac:dyDescent="0.3">
+      <c r="AI34">
+        <f>AN34/AJ34</f>
+        <v>1.8425</v>
+      </c>
+      <c r="AJ34">
+        <v>36</v>
+      </c>
+      <c r="AK34">
+        <f>AI34*6</f>
+        <v>11.055</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <v>36</v>
+      </c>
+      <c r="AN34">
+        <f>SUM(AQ34:AV34)</f>
+        <v>66.33</v>
+      </c>
+      <c r="AO34">
+        <f>$AN$33-SUM($AN$34:AN34)</f>
+        <v>134.67000000000002</v>
+      </c>
+      <c r="AQ34">
+        <f>AN33*1.1 * AJ34/120</f>
+        <v>66.33</v>
+      </c>
+    </row>
+    <row r="35" spans="35:45" x14ac:dyDescent="0.3">
+      <c r="AI35">
+        <f t="shared" ref="AI35:AI36" si="4">AN35/AJ35</f>
+        <v>1.3627321428571431</v>
+      </c>
+      <c r="AJ35">
+        <v>54</v>
+      </c>
+      <c r="AK35">
+        <f t="shared" ref="AK35:AK36" si="5">AI35*6</f>
+        <v>8.1763928571428579</v>
+      </c>
+      <c r="AL35">
+        <v>36</v>
+      </c>
+      <c r="AM35">
+        <v>90</v>
+      </c>
+      <c r="AN35">
+        <f>SUM(AR35:AV35)</f>
+        <v>73.587535714285721</v>
+      </c>
+      <c r="AO35">
+        <f>$AN$33-SUM($AN$34:AN35)</f>
+        <v>61.082464285714281</v>
+      </c>
+      <c r="AR35">
+        <f>AO34*0.85*54/84</f>
+        <v>73.587535714285721</v>
+      </c>
+    </row>
+    <row r="36" spans="35:45" x14ac:dyDescent="0.3">
+      <c r="AI36">
+        <f t="shared" si="4"/>
+        <v>2.0360821428571425</v>
+      </c>
+      <c r="AJ36">
+        <v>30</v>
+      </c>
+      <c r="AK36">
+        <f t="shared" si="5"/>
+        <v>12.216492857142855</v>
+      </c>
+      <c r="AL36">
+        <v>90</v>
+      </c>
+      <c r="AM36">
+        <v>120</v>
+      </c>
+      <c r="AN36">
+        <f t="shared" ref="AN36" si="6">SUM(AQ36:AV36)</f>
+        <v>61.082464285714281</v>
+      </c>
+      <c r="AO36">
+        <f>$AN$33-SUM($AN$34:AN36)</f>
+        <v>0</v>
+      </c>
+      <c r="AS36">
+        <f>AO35</f>
+        <v>61.082464285714281</v>
+      </c>
+    </row>
+    <row r="43" spans="35:45" x14ac:dyDescent="0.3">
+      <c r="AM43">
+        <v>107.2</v>
+      </c>
+      <c r="AN43">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="35:45" x14ac:dyDescent="0.3">
+      <c r="AN44">
+        <v>54</v>
+      </c>
+      <c r="AO44">
+        <f>54*AM43/AN43</f>
+        <v>68.914285714285711</v>
       </c>
     </row>
   </sheetData>
@@ -3704,11 +3817,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E5E5E3-A50C-4051-A74D-79D3C39ABDB7}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D8F7A9-049B-47D3-943A-D6164EAC2EA2}">
   <dimension ref="A1:AB302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31498,12 +31651,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBA5CD5-14A2-45D2-BBA0-8F4D5C460A33}">
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32110,12 +32263,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033AA04C-540B-491B-ADAC-EC2A17DBB7DE}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K22"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32898,11 +33051,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0255C5F8-075F-477D-9280-7CA9953580F8}">
   <dimension ref="A1:Z121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>

</xml_diff>